<commit_message>
Bổ sung code thu thập dữ liệu, Dataset Project 2
</commit_message>
<xml_diff>
--- a/Dataset/Project_1_dataset.xlsx
+++ b/Dataset/Project_1_dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thean\Documents\Social_Network\Social_Network_Projects\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thean\Documents\Social_Network\Social_Network_Projects\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5E961E-2C8C-4CDB-AF79-7115A0EFB651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB68BD8-26C5-4388-BE8D-120E08ABCC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28123,12 +28123,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2050" workbookViewId="0">
+      <selection activeCell="A2076" sqref="A2076"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.44140625" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
+    <col min="2" max="2" width="65.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>